<commit_message>
Add flash modules, MCU, and usb-c receptacle
</commit_message>
<xml_diff>
--- a/display_controller/display_controller_BOM.xlsx
+++ b/display_controller/display_controller_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\DigitalDisplay\display_controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC43F4E5-98D8-497E-B6F5-E83665D70E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A26701-A350-4A6D-A0C6-10AE23D9D49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Item</t>
   </si>
@@ -75,21 +75,6 @@
     <t>Display Connector</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/cvilux-usa/CF31401D0R0-05-NH/15793184</t>
-  </si>
-  <si>
-    <t>Cvilux USA</t>
-  </si>
-  <si>
-    <t>CF31401D0R0-05-NH</t>
-  </si>
-  <si>
-    <t>2987-CF31401D0R0-05-NHCT-ND</t>
-  </si>
-  <si>
-    <t>CONN FFC BOTTOM 40POS 0.5MM R/A</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -117,10 +102,94 @@
     <t>Datasheet</t>
   </si>
   <si>
-    <t>https://www.cvilux.com/uploads/drawings/101/073/CF3103S.pdf</t>
-  </si>
-  <si>
     <t>https://www.ti.com/general/docs/suppproductinfo.tsp?distId=10&amp;gotoUrl=https%3A%2F%2Fwww.ti.com%2Flit%2Fgpn%2Fsn65lvds387</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>4-1734839-0</t>
+  </si>
+  <si>
+    <t>A100229CT-ND</t>
+  </si>
+  <si>
+    <t>CONN FPC TOP 40POS 0.5MM R/A</t>
+  </si>
+  <si>
+    <t>https://www.te.com/usa-en/product-4-1734839-0.datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-amp-connectors/4-1734839-0/2180502</t>
+  </si>
+  <si>
+    <t>Single Picture Flash</t>
+  </si>
+  <si>
+    <t>Data Transfer MCU</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 512KB FLASH 64LQFP</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>STM32F412RET6TR</t>
+  </si>
+  <si>
+    <t>497-19350-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.st.com/content/ccc/resource/technical/document/datasheet/15/90/07/b3/8c/10/4e/95/DM00213872.pdf/files/DM00213872.pdf/jcr:content/translations/en.DM00213872.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/STM32F412RET6TR/6621741?s=N4IgTCBcDaIMoBUCyBmMAxALARjAJQFEEA2BPEAXQF8g</t>
+  </si>
+  <si>
+    <t>USB-C Receptacle</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>CONN RCP USB2.0 TYP C 24P SMD RA</t>
+  </si>
+  <si>
+    <t>GCT</t>
+  </si>
+  <si>
+    <t>USB4105-GF-A-120</t>
+  </si>
+  <si>
+    <t>2073-USB4105-GF-A-120CT-ND</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/5702/USB4105%20-%20Product%20Drawing.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/gct/USB4105-GF-A-120/14559037</t>
+  </si>
+  <si>
+    <t>IC FLASH 16MBIT SPI/QUAD 8SOP</t>
+  </si>
+  <si>
+    <t>GigaDevice Semiconductor (HK) Limited</t>
+  </si>
+  <si>
+    <t>GD25Q16ETIGR</t>
+  </si>
+  <si>
+    <t>1970-GD25Q16ETIGRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.gigadevice.com.cn/Public/Uploads/uploadfile/files/20220714/DS-00473-GD25Q16E-Rev1.2.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/gigadevice-semiconductor-hk-limited/GD25Q16ETIGR/14113855</t>
   </si>
 </sst>
 </file>
@@ -236,7 +305,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -249,18 +318,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -554,7 +621,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,7 +631,7 @@
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="11.21875" customWidth="1"/>
     <col min="5" max="5" width="34.109375" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
     <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.21875" customWidth="1"/>
     <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
@@ -574,13 +641,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -591,11 +658,11 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -607,7 +674,7 @@
       </c>
       <c r="M2" s="7">
         <f>SUM(M4:M24)</f>
-        <v>3.4000000000000004</v>
+        <v>20.239999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -639,13 +706,13 @@
         <v>9</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>10</v>
@@ -660,40 +727,40 @@
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>18</v>
+        <v>29</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="14" t="s">
+      <c r="I4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>16</v>
+      <c r="K4" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="L4" s="11">
-        <v>0.43</v>
+        <v>1.03</v>
       </c>
       <c r="M4" s="11">
-        <f>B4*L4</f>
-        <v>0.43</v>
+        <f t="shared" ref="M4:M24" si="0">B4*L4</f>
+        <v>1.03</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B5" s="10">
         <v>1</v>
@@ -703,86 +770,150 @@
         <v>14</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>26</v>
+      <c r="K5" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="L5" s="11">
         <v>2.97</v>
       </c>
       <c r="M5" s="11">
-        <f>B5*L5</f>
+        <f t="shared" si="0"/>
         <v>2.97</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="10">
+        <v>8</v>
+      </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="11"/>
+      <c r="E6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0.72</v>
+      </c>
       <c r="M6" s="11">
-        <f>B6*L6</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.76</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="11"/>
+      <c r="D7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="11">
+        <v>9.67</v>
+      </c>
       <c r="M7" s="11">
-        <f>B7*L7</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.67</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="11"/>
+      <c r="D8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0.81</v>
+      </c>
       <c r="M8" s="11">
-        <f>B8*L8</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.81</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -791,15 +922,15 @@
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="10"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11">
-        <f>B9*L9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -809,15 +940,15 @@
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="12"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11">
-        <f>B10*L10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -827,15 +958,15 @@
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="12"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11">
-        <f>B11*L11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -845,15 +976,15 @@
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11">
-        <f>B12*L12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -863,15 +994,15 @@
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="12"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="11"/>
       <c r="M13" s="11">
-        <f>B13*L13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -881,15 +1012,15 @@
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
       <c r="L14" s="11"/>
       <c r="M14" s="11">
-        <f>B14*L14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -899,15 +1030,15 @@
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="12"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11">
-        <f>B15*L15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -917,15 +1048,15 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11">
-        <f>B16*L16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -935,15 +1066,15 @@
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11">
-        <f>B17*L17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -953,15 +1084,15 @@
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="10"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11">
-        <f>B18*L18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -971,15 +1102,15 @@
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11">
-        <f>B19*L19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -989,15 +1120,15 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="12"/>
       <c r="H20" s="10"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11">
-        <f>B20*L20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1007,15 +1138,15 @@
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="12"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
       <c r="L21" s="11"/>
       <c r="M21" s="11">
-        <f>B21*L21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1025,15 +1156,15 @@
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
       <c r="L22" s="11"/>
       <c r="M22" s="11">
-        <f>B22*L22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1043,15 +1174,15 @@
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="12"/>
       <c r="H23" s="10"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
       <c r="L23" s="11"/>
       <c r="M23" s="11">
-        <f>B23*L23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1061,15 +1192,15 @@
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
       <c r="L24" s="11"/>
       <c r="M24" s="11">
-        <f>B24*L24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1083,9 +1214,11 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="K4" r:id="rId1" xr:uid="{FE481A3B-890B-4668-81F9-5405E4141E7B}"/>
-    <hyperlink ref="K5" r:id="rId2" xr:uid="{12318924-7704-4A2C-A19B-33F85B083D9A}"/>
+    <hyperlink ref="K5" r:id="rId1" xr:uid="{12318924-7704-4A2C-A19B-33F85B083D9A}"/>
+    <hyperlink ref="K7" r:id="rId2" xr:uid="{9CB5F883-5008-4413-A693-48AC4AA6D200}"/>
+    <hyperlink ref="K8" r:id="rId3" xr:uid="{D727A0CA-1D5F-45EC-8E2E-ABB82EBA5614}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>